<commit_message>
New excel files, added proper config filenames to test.
</commit_message>
<xml_diff>
--- a/ClueBoard/ClueBoard.xlsx
+++ b/ClueBoard/ClueBoard.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -179,7 +179,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="126">
+  <dxfs count="74">
     <dxf>
       <font>
         <sz val="11"/>
@@ -202,6 +202,19 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
+          <bgColor rgb="FFE46C0A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF558ED5"/>
         </patternFill>
       </fill>
@@ -267,6 +280,32 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFE46C0A"/>
         </patternFill>
       </fill>
@@ -319,6 +358,32 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE46C0A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF558ED5"/>
         </patternFill>
       </fill>
@@ -332,6 +397,84 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -345,6 +488,45 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFE46C0A"/>
         </patternFill>
       </fill>
@@ -397,6 +579,32 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE46C0A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF558ED5"/>
         </patternFill>
       </fill>
@@ -410,6 +618,97 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE46C0A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -423,6 +722,32 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFE46C0A"/>
         </patternFill>
       </fill>
@@ -475,6 +800,32 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE46C0A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF558ED5"/>
         </patternFill>
       </fill>
@@ -488,7 +839,20 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF558ED5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -515,1046 +879,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4016,35 +3340,35 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="S12">
-    <cfRule type="containsText" dxfId="125" priority="2" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="124" priority="3" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="123" priority="4" operator="containsText" text="R"/>
-    <cfRule type="cellIs" dxfId="122" priority="5" operator="equal">
+    <cfRule type="containsText" dxfId="73" priority="2" operator="containsText" text="D"/>
+    <cfRule type="containsText" dxfId="72" priority="3" operator="containsText" text="U"/>
+    <cfRule type="containsText" dxfId="71" priority="4" operator="containsText" text="R"/>
+    <cfRule type="cellIs" dxfId="70" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="6" operator="equal">
       <formula>"W"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S11">
-    <cfRule type="containsText" dxfId="120" priority="7" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="119" priority="8" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="118" priority="9" operator="containsText" text="R"/>
-    <cfRule type="cellIs" dxfId="117" priority="10" operator="equal">
+    <cfRule type="containsText" dxfId="68" priority="7" operator="containsText" text="D"/>
+    <cfRule type="containsText" dxfId="67" priority="8" operator="containsText" text="U"/>
+    <cfRule type="containsText" dxfId="66" priority="9" operator="containsText" text="R"/>
+    <cfRule type="cellIs" dxfId="65" priority="10" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="11" operator="equal">
       <formula>"W"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="12" operator="containsText" text="L"/>
+    <cfRule type="containsText" dxfId="63" priority="12" operator="containsText" text="L"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:W23">
-    <cfRule type="containsText" dxfId="114" priority="13" operator="containsText" text="W"/>
-    <cfRule type="containsText" dxfId="113" priority="14" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="112" priority="15" operator="containsText" text="L"/>
-    <cfRule type="containsText" dxfId="111" priority="16" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="110" priority="17" operator="containsText" text="R"/>
-    <cfRule type="containsText" dxfId="109" priority="18" operator="containsText" text="X"/>
+    <cfRule type="containsText" dxfId="62" priority="13" operator="containsText" text="W"/>
+    <cfRule type="containsText" dxfId="61" priority="14" operator="containsText" text="D"/>
+    <cfRule type="containsText" dxfId="60" priority="15" operator="containsText" text="L"/>
+    <cfRule type="containsText" dxfId="59" priority="16" operator="containsText" text="U"/>
+    <cfRule type="containsText" dxfId="58" priority="17" operator="containsText" text="R"/>
+    <cfRule type="containsText" dxfId="57" priority="18" operator="containsText" text="X"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4056,7 +3380,7 @@
   <dimension ref="A1:X51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7612,67 +6936,56 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="S12">
-    <cfRule type="containsText" dxfId="108" priority="18" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="107" priority="19" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="106" priority="20" operator="containsText" text="R"/>
-    <cfRule type="cellIs" dxfId="105" priority="21" operator="equal">
+  <conditionalFormatting sqref="A1:W23">
+    <cfRule type="containsText" dxfId="0" priority="34" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="W">
+      <formula>NOT(ISERROR(SEARCH("W",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="D">
+      <formula>NOT(ISERROR(SEARCH("D",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="U">
+      <formula>NOT(ISERROR(SEARCH("U",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="25" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="28" operator="containsText" text="L">
+      <formula>NOT(ISERROR(SEARCH("L",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S39">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="D"/>
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="U"/>
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="R"/>
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="22" operator="equal">
-      <formula>"W"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
-    <cfRule type="containsText" dxfId="98" priority="23" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="97" priority="24" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="96" priority="25" operator="containsText" text="R"/>
-    <cfRule type="cellIs" dxfId="95" priority="26" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="27" operator="equal">
-      <formula>"W"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="28" operator="containsText" text="L"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W23">
-    <cfRule type="containsText" dxfId="86" priority="29" operator="containsText" text="W"/>
-    <cfRule type="containsText" dxfId="85" priority="30" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="84" priority="31" operator="containsText" text="L"/>
-    <cfRule type="containsText" dxfId="83" priority="32" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="82" priority="33" operator="containsText" text="R"/>
-    <cfRule type="containsText" dxfId="81" priority="34" operator="containsText" text="X"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S39">
-    <cfRule type="containsText" dxfId="57" priority="1" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="56" priority="2" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="55" priority="3" operator="containsText" text="R"/>
-    <cfRule type="cellIs" dxfId="54" priority="4" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"W"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S38">
-    <cfRule type="containsText" dxfId="47" priority="6" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="46" priority="7" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="45" priority="8" operator="containsText" text="R"/>
-    <cfRule type="cellIs" dxfId="44" priority="9" operator="equal">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="D"/>
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="U"/>
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="R"/>
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"W"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="11" operator="containsText" text="L"/>
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="L"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:W50">
-    <cfRule type="containsText" dxfId="35" priority="12" operator="containsText" text="W"/>
-    <cfRule type="containsText" dxfId="34" priority="13" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="33" priority="14" operator="containsText" text="L"/>
-    <cfRule type="containsText" dxfId="32" priority="15" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="31" priority="16" operator="containsText" text="R"/>
-    <cfRule type="containsText" dxfId="30" priority="17" operator="containsText" text="X"/>
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="W"/>
+    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="D"/>
+    <cfRule type="containsText" dxfId="4" priority="14" operator="containsText" text="L"/>
+    <cfRule type="containsText" dxfId="3" priority="15" operator="containsText" text="U"/>
+    <cfRule type="containsText" dxfId="2" priority="16" operator="containsText" text="R"/>
+    <cfRule type="containsText" dxfId="1" priority="17" operator="containsText" text="X"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Test annotated clue board.
</commit_message>
<xml_diff>
--- a/ClueBoard/ClueBoard.xlsx
+++ b/ClueBoard/ClueBoard.xlsx
@@ -179,20 +179,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="74">
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="40">
     <dxf>
       <font>
         <sz val="11"/>
@@ -488,436 +475,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF558ED5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3340,35 +2898,35 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="S12">
-    <cfRule type="containsText" dxfId="73" priority="2" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="72" priority="3" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="71" priority="4" operator="containsText" text="R"/>
-    <cfRule type="cellIs" dxfId="70" priority="5" operator="equal">
+    <cfRule type="containsText" dxfId="39" priority="2" operator="containsText" text="D"/>
+    <cfRule type="containsText" dxfId="38" priority="3" operator="containsText" text="U"/>
+    <cfRule type="containsText" dxfId="37" priority="4" operator="containsText" text="R"/>
+    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
       <formula>"W"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S11">
-    <cfRule type="containsText" dxfId="68" priority="7" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="67" priority="8" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="66" priority="9" operator="containsText" text="R"/>
-    <cfRule type="cellIs" dxfId="65" priority="10" operator="equal">
+    <cfRule type="containsText" dxfId="34" priority="7" operator="containsText" text="D"/>
+    <cfRule type="containsText" dxfId="33" priority="8" operator="containsText" text="U"/>
+    <cfRule type="containsText" dxfId="32" priority="9" operator="containsText" text="R"/>
+    <cfRule type="cellIs" dxfId="31" priority="10" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="11" operator="equal">
       <formula>"W"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="12" operator="containsText" text="L"/>
+    <cfRule type="containsText" dxfId="29" priority="12" operator="containsText" text="L"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:W23">
-    <cfRule type="containsText" dxfId="62" priority="13" operator="containsText" text="W"/>
-    <cfRule type="containsText" dxfId="61" priority="14" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="60" priority="15" operator="containsText" text="L"/>
-    <cfRule type="containsText" dxfId="59" priority="16" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="58" priority="17" operator="containsText" text="R"/>
-    <cfRule type="containsText" dxfId="57" priority="18" operator="containsText" text="X"/>
+    <cfRule type="containsText" dxfId="28" priority="13" operator="containsText" text="W"/>
+    <cfRule type="containsText" dxfId="27" priority="14" operator="containsText" text="D"/>
+    <cfRule type="containsText" dxfId="26" priority="15" operator="containsText" text="L"/>
+    <cfRule type="containsText" dxfId="25" priority="16" operator="containsText" text="U"/>
+    <cfRule type="containsText" dxfId="24" priority="17" operator="containsText" text="R"/>
+    <cfRule type="containsText" dxfId="23" priority="18" operator="containsText" text="X"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3380,7 +2938,7 @@
   <dimension ref="A1:X51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA21" sqref="AA21"/>
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6937,55 +6495,55 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:W23">
-    <cfRule type="containsText" dxfId="0" priority="34" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="22" priority="34" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="U">
+    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="U">
       <formula>NOT(ISERROR(SEARCH("U",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="25" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="18" priority="25" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="28" operator="containsText" text="L">
+    <cfRule type="containsText" dxfId="17" priority="28" operator="containsText" text="L">
       <formula>NOT(ISERROR(SEARCH("L",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S39">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="R"/>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="D"/>
+    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="U"/>
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="R"/>
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"W"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S38">
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="R"/>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="D"/>
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="U"/>
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="R"/>
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>"W"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="L"/>
+    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="L"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:W50">
-    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="W"/>
-    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="D"/>
-    <cfRule type="containsText" dxfId="4" priority="14" operator="containsText" text="L"/>
-    <cfRule type="containsText" dxfId="3" priority="15" operator="containsText" text="U"/>
-    <cfRule type="containsText" dxfId="2" priority="16" operator="containsText" text="R"/>
-    <cfRule type="containsText" dxfId="1" priority="17" operator="containsText" text="X"/>
+    <cfRule type="containsText" dxfId="5" priority="12" operator="containsText" text="W"/>
+    <cfRule type="containsText" dxfId="4" priority="13" operator="containsText" text="D"/>
+    <cfRule type="containsText" dxfId="3" priority="14" operator="containsText" text="L"/>
+    <cfRule type="containsText" dxfId="2" priority="15" operator="containsText" text="U"/>
+    <cfRule type="containsText" dxfId="1" priority="16" operator="containsText" text="R"/>
+    <cfRule type="containsText" dxfId="0" priority="17" operator="containsText" text="X"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>